<commit_message>
update with corrected HK-60 RNA-seq
</commit_message>
<xml_diff>
--- a/combined_analysis/intersectional-genes/Rho_up & Exp_down & Hyper_m6A.xlsx
+++ b/combined_analysis/intersectional-genes/Rho_up & Exp_down & Hyper_m6A.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="62">
   <si>
     <t>chr</t>
   </si>
@@ -63,58 +63,67 @@
     <t>ensembl</t>
   </si>
   <si>
-    <t>chr15</t>
+    <t>chr3</t>
+  </si>
+  <si>
+    <t>chr17</t>
   </si>
   <si>
     <t>chr19</t>
   </si>
   <si>
-    <t>chr12</t>
-  </si>
-  <si>
-    <t>chr16</t>
-  </si>
-  <si>
-    <t>CEP152</t>
-  </si>
-  <si>
-    <t>MAP1S</t>
-  </si>
-  <si>
-    <t>MBD6</t>
-  </si>
-  <si>
-    <t>DDX19A</t>
-  </si>
-  <si>
-    <t>UHRF1</t>
+    <t>chr11</t>
+  </si>
+  <si>
+    <t>chr1</t>
+  </si>
+  <si>
+    <t>EIF4G1</t>
+  </si>
+  <si>
+    <t>SPOP</t>
+  </si>
+  <si>
+    <t>KLF16</t>
+  </si>
+  <si>
+    <t>MRPL17</t>
+  </si>
+  <si>
+    <t>YTHDF2</t>
+  </si>
+  <si>
+    <t>KTI12</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
     <t>49</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>ENSG00000103995.14</t>
-  </si>
-  <si>
-    <t>ENSG00000130479.11</t>
-  </si>
-  <si>
-    <t>ENSG00000166987.15</t>
-  </si>
-  <si>
-    <t>ENSG00000168872.17</t>
-  </si>
-  <si>
-    <t>ENSG00000276043.5</t>
+    <t>ENSG00000114867.21</t>
+  </si>
+  <si>
+    <t>ENSG00000121067.19</t>
+  </si>
+  <si>
+    <t>ENSG00000129911.9</t>
+  </si>
+  <si>
+    <t>ENSG00000158042.9</t>
+  </si>
+  <si>
+    <t>ENSG00000198492.16</t>
+  </si>
+  <si>
+    <t>ENSG00000198841.4</t>
   </si>
   <si>
     <t>Exp.hl60.log2FC</t>
@@ -550,7 +559,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -608,25 +617,25 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>48740562</v>
+        <v>184334762</v>
       </c>
       <c r="C2">
-        <v>48740611</v>
+        <v>184334811</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G2">
-        <v>48740562</v>
+        <v>184334762</v>
       </c>
       <c r="H2">
-        <v>48740611</v>
+        <v>184334811</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -635,30 +644,30 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M2">
-        <v>4.18965474389274</v>
+        <v>6.2461067654722</v>
       </c>
       <c r="N2">
-        <v>0.000449048891393633</v>
+        <v>1.063111376709E-09</v>
       </c>
       <c r="O2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>17726426</v>
+        <v>184335110</v>
       </c>
       <c r="C3">
-        <v>17726475</v>
+        <v>184335159</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -667,13 +676,13 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>17726426</v>
+        <v>184335110</v>
       </c>
       <c r="H3">
-        <v>17726475</v>
+        <v>184335159</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -682,30 +691,30 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M3">
-        <v>3.90197266957464</v>
+        <v>4.93447393312132</v>
       </c>
       <c r="N3">
-        <v>0.00330789341084215</v>
+        <v>7.437631607265509E-07</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>57529354</v>
+        <v>49599828</v>
       </c>
       <c r="C4">
-        <v>57529403</v>
+        <v>49599877</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -714,13 +723,13 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G4">
-        <v>57529354</v>
+        <v>49599828</v>
       </c>
       <c r="H4">
-        <v>57529403</v>
+        <v>49599877</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -729,45 +738,45 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M4">
-        <v>3.70130197395147</v>
+        <v>4.4543472962535</v>
       </c>
       <c r="N4">
-        <v>8.75509795339457E-06</v>
+        <v>0.00390712658675885</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>70372184</v>
+        <v>49599927</v>
       </c>
       <c r="C5">
-        <v>70372233</v>
+        <v>49599976</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G5">
-        <v>70372184</v>
+        <v>49599927</v>
       </c>
       <c r="H5">
-        <v>70372233</v>
+        <v>49599976</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -776,16 +785,16 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M5">
-        <v>1.3028278300968</v>
+        <v>4.55387689160054</v>
       </c>
       <c r="N5">
-        <v>0.0009859978971932251</v>
+        <v>0.00328463648875865</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -793,13 +802,13 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>70372484</v>
+        <v>1854475</v>
       </c>
       <c r="C6">
-        <v>70372533</v>
+        <v>1854524</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -808,13 +817,13 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>70372484</v>
+        <v>1854475</v>
       </c>
       <c r="H6">
-        <v>70372533</v>
+        <v>1854524</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -823,45 +832,45 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M6">
-        <v>1.6259672143853</v>
+        <v>-1.84054963339749</v>
       </c>
       <c r="N6">
-        <v>4.22369666268629E-05</v>
+        <v>0.000273844330500483</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>4961506</v>
+        <v>1854574</v>
       </c>
       <c r="C7">
-        <v>4961555</v>
+        <v>1854623</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G7">
-        <v>4961506</v>
+        <v>1854574</v>
       </c>
       <c r="H7">
-        <v>4961555</v>
+        <v>1854623</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -870,16 +879,16 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M7">
-        <v>1.03027752842571</v>
+        <v>2.96398357523936</v>
       </c>
       <c r="N7">
-        <v>0.000369457620172153</v>
+        <v>0.00435014396607925</v>
       </c>
       <c r="O7" t="s">
         <v>32</v>
@@ -887,13 +896,13 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>4961755</v>
+        <v>6682208</v>
       </c>
       <c r="C8">
-        <v>4961804</v>
+        <v>6682257</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -902,13 +911,13 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G8">
-        <v>4961755</v>
+        <v>6682208</v>
       </c>
       <c r="H8">
-        <v>4961804</v>
+        <v>6682257</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -917,19 +926,254 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8">
+        <v>1.84516024595485</v>
+      </c>
+      <c r="N8">
+        <v>0.000322116124125027</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>28742646</v>
+      </c>
+      <c r="C9">
+        <v>28742695</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="L8" t="s">
+      <c r="G9">
+        <v>28742646</v>
+      </c>
+      <c r="H9">
+        <v>28742695</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9">
+        <v>4.07753744389635</v>
+      </c>
+      <c r="N9">
+        <v>2.29475209302388E-05</v>
+      </c>
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>28742944</v>
+      </c>
+      <c r="C10">
+        <v>28742993</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>28742944</v>
+      </c>
+      <c r="H10">
+        <v>28742993</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10">
+        <v>1.01297046222352</v>
+      </c>
+      <c r="N10">
+        <v>0.000723892314729135</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>28743143</v>
+      </c>
+      <c r="C11">
+        <v>28743192</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <v>28743143</v>
+      </c>
+      <c r="H11">
+        <v>28743192</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11">
+        <v>-0.801795698025198</v>
+      </c>
+      <c r="N11">
+        <v>0.000387026255780798</v>
+      </c>
+      <c r="O11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>52032493</v>
+      </c>
+      <c r="C12">
+        <v>52032542</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="M8">
-        <v>1.73753791506142</v>
-      </c>
-      <c r="N8">
-        <v>0.00073579121568701</v>
-      </c>
-      <c r="O8" t="s">
-        <v>32</v>
+      <c r="G12">
+        <v>52032493</v>
+      </c>
+      <c r="H12">
+        <v>52032542</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12">
+        <v>1.33750419695045</v>
+      </c>
+      <c r="N12">
+        <v>0.00205149734260535</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>52032883</v>
+      </c>
+      <c r="C13">
+        <v>52032932</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13">
+        <v>52032883</v>
+      </c>
+      <c r="H13">
+        <v>52032932</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13">
+        <v>3.34990408718034</v>
+      </c>
+      <c r="N13">
+        <v>0.000340130211492928</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +1183,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -947,269 +1191,328 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>-1.278</v>
+        <v>-0.536</v>
       </c>
       <c r="C2">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.59</v>
+        <v>-0.033</v>
       </c>
       <c r="E2">
-        <v>0.112</v>
+        <v>0.891</v>
       </c>
       <c r="F2">
-        <v>-0.116</v>
+        <v>-0.274</v>
       </c>
       <c r="G2">
-        <v>0.658</v>
+        <v>0.183</v>
       </c>
       <c r="H2">
-        <v>0.168</v>
+        <v>-0.108</v>
       </c>
       <c r="I2">
-        <v>0.569</v>
+        <v>0.583</v>
       </c>
       <c r="J2">
-        <v>-0.113</v>
+        <v>-0.406</v>
       </c>
       <c r="K2">
-        <v>0.705</v>
+        <v>0.035</v>
       </c>
       <c r="L2">
-        <v>-0.281</v>
+        <v>0.097</v>
       </c>
       <c r="M2">
-        <v>0.251</v>
+        <v>0.667</v>
       </c>
       <c r="N2">
-        <v>0.783</v>
+        <v>-0.099</v>
       </c>
       <c r="O2">
-        <v>0.262</v>
+        <v>0.928</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>-0.16</v>
+        <v>-1.046</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D3">
-        <v>-0.204</v>
+        <v>0.048</v>
       </c>
       <c r="E3">
-        <v>0.204</v>
+        <v>0.858</v>
       </c>
       <c r="F3">
-        <v>-0.341</v>
+        <v>-0.354</v>
       </c>
       <c r="G3">
-        <v>0.018</v>
+        <v>0.238</v>
       </c>
       <c r="H3">
-        <v>-0.206</v>
+        <v>0.113</v>
       </c>
       <c r="I3">
-        <v>0.12</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="J3">
-        <v>-0.195</v>
+        <v>-0.36</v>
       </c>
       <c r="K3">
-        <v>0.292</v>
+        <v>0.308</v>
       </c>
       <c r="L3">
-        <v>-0.146</v>
+        <v>-0.433</v>
       </c>
       <c r="M3">
-        <v>0.411</v>
+        <v>0.111</v>
+      </c>
+      <c r="N3">
+        <v>-0.183</v>
+      </c>
+      <c r="O3">
+        <v>0.91</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>-0.067</v>
+        <v>-0.992</v>
       </c>
       <c r="C4">
-        <v>0.022</v>
+        <v>0.046</v>
       </c>
       <c r="D4">
-        <v>-0.497</v>
+        <v>-0.201</v>
       </c>
       <c r="E4">
-        <v>0.044</v>
+        <v>0.468</v>
       </c>
       <c r="F4">
-        <v>-0.106</v>
+        <v>-0.064</v>
       </c>
       <c r="G4">
-        <v>0.661</v>
+        <v>0.85</v>
       </c>
       <c r="H4">
-        <v>0.317</v>
+        <v>-0.108</v>
       </c>
       <c r="I4">
-        <v>0.343</v>
+        <v>0.72</v>
       </c>
       <c r="J4">
-        <v>-0.065</v>
+        <v>-0.356</v>
       </c>
       <c r="K4">
-        <v>0.78</v>
+        <v>0.227</v>
       </c>
       <c r="L4">
-        <v>-0.148</v>
+        <v>0.108</v>
       </c>
       <c r="M4">
-        <v>0.63</v>
+        <v>0.668</v>
       </c>
       <c r="N4">
-        <v>-0.122</v>
+        <v>-0.8080000000000001</v>
       </c>
       <c r="O4">
-        <v>0.914</v>
+        <v>0.365</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>-0.415</v>
+        <v>-0.612</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.021</v>
       </c>
       <c r="D5">
-        <v>-0.07099999999999999</v>
+        <v>-0.178</v>
       </c>
       <c r="E5">
-        <v>0.6830000000000001</v>
+        <v>0.198</v>
       </c>
       <c r="F5">
-        <v>-0.204</v>
+        <v>-0.137</v>
       </c>
       <c r="G5">
-        <v>0.324</v>
+        <v>0.496</v>
       </c>
       <c r="H5">
-        <v>-0.029</v>
+        <v>0.112</v>
       </c>
       <c r="I5">
-        <v>0.885</v>
+        <v>0.58</v>
       </c>
       <c r="J5">
-        <v>-0.031</v>
+        <v>-0.293</v>
       </c>
       <c r="K5">
-        <v>0.891</v>
+        <v>0.365</v>
       </c>
       <c r="L5">
-        <v>0.079</v>
+        <v>-0.093</v>
       </c>
       <c r="M5">
-        <v>0.633</v>
+        <v>0.612</v>
+      </c>
+      <c r="N5">
+        <v>0.457</v>
+      </c>
+      <c r="O5">
+        <v>0.609</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>-3.096</v>
+        <v>-0.24</v>
       </c>
       <c r="C6">
-        <v>0.008</v>
+        <v>0.032</v>
       </c>
       <c r="D6">
-        <v>1.048</v>
+        <v>0.004</v>
       </c>
       <c r="E6">
-        <v>0.13</v>
+        <v>0.977</v>
       </c>
       <c r="F6">
-        <v>-0.441</v>
+        <v>0.278</v>
       </c>
       <c r="G6">
-        <v>0.06</v>
+        <v>0.338</v>
       </c>
       <c r="H6">
-        <v>-0.206</v>
+        <v>-0.33</v>
       </c>
       <c r="I6">
-        <v>0.22</v>
+        <v>0.065</v>
       </c>
       <c r="J6">
-        <v>0.448</v>
+        <v>0.145</v>
       </c>
       <c r="K6">
-        <v>0.707</v>
+        <v>0.55</v>
       </c>
       <c r="L6">
-        <v>-0.119</v>
+        <v>0.305</v>
       </c>
       <c r="M6">
-        <v>0.569</v>
+        <v>0.209</v>
       </c>
       <c r="N6">
-        <v>0.731</v>
+        <v>0.1</v>
       </c>
       <c r="O6">
-        <v>0.151</v>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>-0.37</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-0.177</v>
+      </c>
+      <c r="E7">
+        <v>0.264</v>
+      </c>
+      <c r="F7">
+        <v>0.031</v>
+      </c>
+      <c r="G7">
+        <v>0.826</v>
+      </c>
+      <c r="H7">
+        <v>-0.028</v>
+      </c>
+      <c r="I7">
+        <v>0.801</v>
+      </c>
+      <c r="J7">
+        <v>-0.176</v>
+      </c>
+      <c r="K7">
+        <v>0.261</v>
+      </c>
+      <c r="L7">
+        <v>0.111</v>
+      </c>
+      <c r="M7">
+        <v>0.458</v>
+      </c>
+      <c r="N7">
+        <v>0.276</v>
+      </c>
+      <c r="O7">
+        <v>0.031</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1522,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1230,245 +1533,286 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>0.155</v>
+        <v>0.133</v>
       </c>
       <c r="C2">
-        <v>0.02</v>
+        <v>0.005</v>
       </c>
       <c r="D2">
-        <v>0.113</v>
+        <v>0.26</v>
       </c>
       <c r="E2">
-        <v>0.241</v>
+        <v>0.038</v>
       </c>
       <c r="F2">
-        <v>0.148</v>
+        <v>0.242</v>
       </c>
       <c r="G2">
-        <v>0.427</v>
+        <v>0.023</v>
       </c>
       <c r="H2">
+        <v>-0.105</v>
+      </c>
+      <c r="I2">
         <v>0.055</v>
       </c>
-      <c r="I2">
-        <v>0.153</v>
-      </c>
       <c r="J2">
-        <v>-0.027</v>
+        <v>-0.11</v>
       </c>
       <c r="K2">
-        <v>0.982</v>
+        <v>0.039</v>
       </c>
       <c r="L2">
-        <v>-0.027</v>
+        <v>-0.11</v>
       </c>
       <c r="M2">
-        <v>0.982</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>0.121</v>
+        <v>0.165</v>
       </c>
       <c r="C3">
-        <v>0.043</v>
+        <v>0.005</v>
       </c>
       <c r="D3">
-        <v>0.165</v>
+        <v>0.204</v>
       </c>
       <c r="E3">
-        <v>0.018</v>
+        <v>0.005</v>
       </c>
       <c r="F3">
-        <v>0.411</v>
+        <v>0.283</v>
       </c>
       <c r="G3">
-        <v>0.003</v>
+        <v>0.02</v>
       </c>
       <c r="H3">
-        <v>-0.317</v>
+        <v>-0.06900000000000001</v>
       </c>
       <c r="I3">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
       <c r="J3">
-        <v>-0.493</v>
+        <v>-0.108</v>
       </c>
       <c r="K3">
-        <v>0.005</v>
+        <v>0.103</v>
       </c>
       <c r="L3">
-        <v>-0.493</v>
+        <v>-0.108</v>
       </c>
       <c r="M3">
-        <v>0.005</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>0.156</v>
+        <v>0.372</v>
       </c>
       <c r="C4">
-        <v>0.022</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.11</v>
+        <v>0.288</v>
       </c>
       <c r="E4">
-        <v>0.226</v>
+        <v>0.005</v>
       </c>
       <c r="F4">
-        <v>-0.008999999999999999</v>
+        <v>0.406</v>
       </c>
       <c r="G4">
-        <v>0.831</v>
+        <v>0.008</v>
       </c>
       <c r="H4">
-        <v>-0.004</v>
+        <v>-0.198</v>
       </c>
       <c r="I4">
-        <v>0.405</v>
+        <v>0.002</v>
       </c>
       <c r="J4">
-        <v>0.017</v>
+        <v>-0.547</v>
       </c>
       <c r="K4">
-        <v>0.677</v>
+        <v>0.001</v>
       </c>
       <c r="L4">
-        <v>0.017</v>
+        <v>-0.547</v>
       </c>
       <c r="M4">
-        <v>0.677</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>0.16</v>
+        <v>0.118</v>
       </c>
       <c r="C5">
-        <v>0.078</v>
+        <v>0.036</v>
       </c>
       <c r="D5">
-        <v>0.214</v>
+        <v>0.238</v>
       </c>
       <c r="E5">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="F5">
-        <v>0.116</v>
+        <v>0.38</v>
       </c>
       <c r="G5">
-        <v>0.294</v>
+        <v>0.001</v>
       </c>
       <c r="H5">
-        <v>0.011</v>
+        <v>-0.066</v>
       </c>
       <c r="I5">
-        <v>0.546</v>
+        <v>0.004</v>
       </c>
       <c r="J5">
-        <v>-0.08</v>
+        <v>-0.2</v>
       </c>
       <c r="K5">
-        <v>0.187</v>
+        <v>0.01</v>
       </c>
       <c r="L5">
-        <v>-0.08</v>
+        <v>-0.2</v>
       </c>
       <c r="M5">
-        <v>0.187</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>0.181</v>
+        <v>0.208</v>
       </c>
       <c r="C6">
-        <v>0.024</v>
+        <v>0.001</v>
       </c>
       <c r="D6">
-        <v>0.123</v>
+        <v>0.274</v>
       </c>
       <c r="E6">
-        <v>0.744</v>
+        <v>0.002</v>
       </c>
       <c r="F6">
-        <v>0.175</v>
+        <v>0.324</v>
       </c>
       <c r="G6">
-        <v>0.208</v>
+        <v>0.004</v>
       </c>
       <c r="H6">
-        <v>-0.194</v>
+        <v>-0.093</v>
       </c>
       <c r="I6">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="J6">
-        <v>-0.231</v>
+        <v>-0.159</v>
       </c>
       <c r="K6">
-        <v>0.006</v>
+        <v>0.03</v>
       </c>
       <c r="L6">
-        <v>-0.231</v>
+        <v>-0.159</v>
       </c>
       <c r="M6">
-        <v>0.006</v>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>0.136</v>
+      </c>
+      <c r="C7">
+        <v>0.016</v>
+      </c>
+      <c r="D7">
+        <v>0.239</v>
+      </c>
+      <c r="E7">
+        <v>0.018</v>
+      </c>
+      <c r="F7">
+        <v>0.431</v>
+      </c>
+      <c r="G7">
+        <v>0.028</v>
+      </c>
+      <c r="H7">
+        <v>-0.117</v>
+      </c>
+      <c r="I7">
+        <v>0.014</v>
+      </c>
+      <c r="J7">
+        <v>-0.151</v>
+      </c>
+      <c r="K7">
+        <v>0.033</v>
+      </c>
+      <c r="L7">
+        <v>-0.151</v>
+      </c>
+      <c r="M7">
+        <v>0.033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>